<commit_message>
fix bomb; fix base class; add food base
修复炸弹不爆炸的问题；为编辑器基类拓展到了子类；新增食物基类功能
</commit_message>
<xml_diff>
--- a/Assets/配置表/Excels/foods.xlsx
+++ b/Assets/配置表/Excels/foods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProjects\GGJ2024\Assets\配置表\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3E5DD2-6825-4952-834E-5A51ED3C556E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C97359B-ADBA-421E-9ED2-9C92DE2C1273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="276" yWindow="2340" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>-5</v>

</xml_diff>